<commit_message>
stripslashes for JSON error
stripslashes for JSON object which occurs in some environments. handled errors if loaded file doesn't exists. changed include paths to work if paths do not resolve to document root correctly
</commit_message>
<xml_diff>
--- a/userdata/data.xlsx
+++ b/userdata/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -97,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,122 +478,462 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>36436</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.51523148148148146</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
-        <v>38812</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.48107638888888887</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3">
-        <v>37623</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.29009259259259262</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3">
-        <v>38415</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.98982638888888896</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>35</v>
-      </c>
-    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>39208</v>
+        <v>36436</v>
       </c>
       <c r="C9" s="1">
-        <v>0.55858796296296298</v>
+        <v>0.51523148148148146</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>40002</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.19027777777777777</v>
+        <v>38812</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.48107638888888887</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>37623</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.29009259259259262</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>38415</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.98982638888888896</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3">
+        <v>39208</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.55858796296296298</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>40002</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.19027777777777777</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B15" s="3">
         <v>40399</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C15" s="2">
         <v>0.62916666666666665</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11">
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <v>41124</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3">
+        <v>40305</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4.5763888888888889E-2</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3">
+        <v>39910</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3">
+        <v>36436</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.51523148148148146</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3">
+        <v>38812</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.48107638888888887</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3">
+        <v>37623</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.29009259259259262</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="3">
+        <v>38415</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.98982638888888896</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3">
+        <v>39208</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.55858796296296298</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3">
+        <v>40002</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.19027777777777777</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3">
+        <v>40399</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3">
+        <v>41124</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3">
+        <v>40305</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4.5763888888888889E-2</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3">
+        <v>39910</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3">
+        <v>36436</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.51523148148148146</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="3">
+        <v>38812</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.48107638888888887</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="3">
+        <v>37623</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.29009259259259262</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="3">
+        <v>38415</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.98982638888888896</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3">
+        <v>39208</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.55858796296296298</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3">
+        <v>40002</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.19027777777777777</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="3">
+        <v>40399</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
getColumnDataTypes time and date fix
can more accurately guess if the data is a date or time, but the code is sloppy.
</commit_message>
<xml_diff>
--- a/userdata/data.xlsx
+++ b/userdata/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Tim</t>
+  </si>
+  <si>
+    <t>1PM</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,8 +437,8 @@
       <c r="B2" s="3">
         <v>41124</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.51736111111111105</v>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
hidden columns are removed
hidden columns are removed from excel sheets before processing them. there is still an error in this process, and the data type of the hidden column is still displayed.
code to handle multiple sheets is being made
</commit_message>
<xml_diff>
--- a/userdata/data.xlsx
+++ b/userdata/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>HiddenStuff</t>
-  </si>
-  <si>
-    <t>Secret Stuff</t>
   </si>
 </sst>
 </file>
@@ -410,14 +407,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -456,8 +455,8 @@
       <c r="E2">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -476,8 +475,8 @@
       <c r="E3">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
-        <v>15</v>
+      <c r="F3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -496,8 +495,8 @@
       <c r="E4">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
-        <v>15</v>
+      <c r="F4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -516,8 +515,8 @@
       <c r="E5">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="F5">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -536,8 +535,8 @@
       <c r="E6">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
-        <v>15</v>
+      <c r="F6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,8 +555,8 @@
       <c r="E7">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
-        <v>15</v>
+      <c r="F7">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,8 +575,8 @@
       <c r="E8">
         <v>35</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
+      <c r="F8">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -596,8 +595,8 @@
       <c r="E9">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
-        <v>15</v>
+      <c r="F9">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -616,8 +615,8 @@
       <c r="E10">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
-        <v>15</v>
+      <c r="F10">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -636,8 +635,8 @@
       <c r="E11">
         <v>60</v>
       </c>
-      <c r="F11" t="s">
-        <v>15</v>
+      <c r="F11">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -656,8 +655,8 @@
       <c r="E12">
         <v>12</v>
       </c>
-      <c r="F12" t="s">
-        <v>15</v>
+      <c r="F12">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -676,8 +675,8 @@
       <c r="E13">
         <v>15</v>
       </c>
-      <c r="F13" t="s">
-        <v>15</v>
+      <c r="F13">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,8 +695,8 @@
       <c r="E14">
         <v>18</v>
       </c>
-      <c r="F14" t="s">
-        <v>15</v>
+      <c r="F14">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,8 +715,8 @@
       <c r="E15">
         <v>21</v>
       </c>
-      <c r="F15" t="s">
-        <v>15</v>
+      <c r="F15">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,7 +735,7 @@
       <c r="E16">
         <v>25</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16">
         <v>15</v>
       </c>
     </row>
@@ -756,8 +755,8 @@
       <c r="E17">
         <v>30</v>
       </c>
-      <c r="F17" t="s">
-        <v>15</v>
+      <c r="F17">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,8 +775,8 @@
       <c r="E18">
         <v>35</v>
       </c>
-      <c r="F18" t="s">
-        <v>15</v>
+      <c r="F18">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,8 +795,8 @@
       <c r="E19">
         <v>40</v>
       </c>
-      <c r="F19" t="s">
-        <v>15</v>
+      <c r="F19">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,8 +815,8 @@
       <c r="E20">
         <v>50</v>
       </c>
-      <c r="F20" t="s">
-        <v>15</v>
+      <c r="F20">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -836,8 +835,8 @@
       <c r="E21">
         <v>60</v>
       </c>
-      <c r="F21" t="s">
-        <v>15</v>
+      <c r="F21">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -856,8 +855,8 @@
       <c r="E22">
         <v>12</v>
       </c>
-      <c r="F22" t="s">
-        <v>15</v>
+      <c r="F22">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -876,8 +875,8 @@
       <c r="E23">
         <v>15</v>
       </c>
-      <c r="F23" t="s">
-        <v>15</v>
+      <c r="F23">
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,8 +895,8 @@
       <c r="E24">
         <v>18</v>
       </c>
-      <c r="F24" t="s">
-        <v>15</v>
+      <c r="F24">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,8 +915,8 @@
       <c r="E25">
         <v>21</v>
       </c>
-      <c r="F25" t="s">
-        <v>15</v>
+      <c r="F25">
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -936,8 +935,8 @@
       <c r="E26">
         <v>25</v>
       </c>
-      <c r="F26" t="s">
-        <v>15</v>
+      <c r="F26">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -956,8 +955,8 @@
       <c r="E27">
         <v>30</v>
       </c>
-      <c r="F27" t="s">
-        <v>15</v>
+      <c r="F27">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -976,8 +975,8 @@
       <c r="E28">
         <v>35</v>
       </c>
-      <c r="F28" t="s">
-        <v>15</v>
+      <c r="F28">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -996,8 +995,8 @@
       <c r="E29">
         <v>40</v>
       </c>
-      <c r="F29" t="s">
-        <v>15</v>
+      <c r="F29">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,8 +1015,8 @@
       <c r="E30">
         <v>50</v>
       </c>
-      <c r="F30" t="s">
-        <v>15</v>
+      <c r="F30">
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1036,8 +1035,8 @@
       <c r="E31">
         <v>60</v>
       </c>
-      <c r="F31" t="s">
-        <v>15</v>
+      <c r="F31">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>